<commit_message>
Published state of ETDataset for deploy May 2025
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy/energy_flexibility_flow_batteries_electricity.xlsx
+++ b/nodes_source_analyses/energy/energy/energy_flexibility_flow_batteries_electricity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10402"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roosdekok/code/etdataset/nodes_source_analyses/energy/energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyradehaan/github/etdataset/nodes_source_analyses/energy/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DC7163-2397-0F43-8226-BA90C22D6D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C21E67-F542-1C4D-B6F6-8A5CD79E9F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" tabRatio="762" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5740" yWindow="-21600" windowWidth="38400" windowHeight="21600" tabRatio="762" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="120">
   <si>
     <t>Source</t>
   </si>
@@ -306,9 +306,6 @@
     <t>typical_input_capacity</t>
   </si>
   <si>
-    <t>Mathijs Bijkerk</t>
-  </si>
-  <si>
     <t>Elestor</t>
   </si>
   <si>
@@ -430,6 +427,12 @@
   </si>
   <si>
     <t>energy_flexibility_flow_batteries_electricity.ad</t>
+  </si>
+  <si>
+    <t>Quintel assumption: output capacity is the same as input capacity</t>
+  </si>
+  <si>
+    <t>Kyra de Haan</t>
   </si>
 </sst>
 </file>
@@ -2291,7 +2294,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
@@ -2326,7 +2329,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="140" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2335,7 +2338,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2494,8 +2497,8 @@
   </sheetPr>
   <dimension ref="B2:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScale="109" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16" customHeight="1"/>
@@ -2616,7 +2619,7 @@
         <v>66</v>
       </c>
       <c r="D11" s="97" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11" s="94">
         <f>'Research data'!E7</f>
@@ -2644,7 +2647,7 @@
       </c>
       <c r="F12" s="95"/>
       <c r="G12" s="146" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I12" s="123" t="str">
         <f>'Research data'!I10</f>
@@ -2662,13 +2665,13 @@
       </c>
       <c r="E13" s="94">
         <f>'Research data'!E9</f>
-        <v>190</v>
+        <v>380</v>
       </c>
       <c r="F13" s="95"/>
       <c r="G13" s="96"/>
       <c r="I13" s="123" t="str">
         <f>'Research data'!I9</f>
-        <v>Expert estimate by Elestor: average of range</v>
+        <v>Quintel assumption: output capacity is the same as input capacity</v>
       </c>
       <c r="J13" s="83"/>
     </row>
@@ -2706,7 +2709,7 @@
       <c r="F15" s="95"/>
       <c r="G15" s="95"/>
       <c r="I15" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J15" s="85"/>
     </row>
@@ -2724,7 +2727,7 @@
       <c r="F16" s="95"/>
       <c r="G16" s="95"/>
       <c r="I16" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J16" s="85"/>
     </row>
@@ -2742,7 +2745,7 @@
       <c r="F17" s="95"/>
       <c r="G17" s="95"/>
       <c r="I17" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J17" s="85"/>
     </row>
@@ -2776,17 +2779,17 @@
       <c r="F20" s="95"/>
       <c r="G20" s="95"/>
       <c r="I20" s="147" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J20" s="85"/>
     </row>
     <row r="21" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B21" s="84"/>
       <c r="C21" s="146" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D21" s="97" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E21" s="98">
         <f>'Research data'!E13</f>
@@ -2803,10 +2806,10 @@
     <row r="22" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B22" s="84"/>
       <c r="C22" s="146" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D22" s="97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" s="98">
         <f>'Research data'!E14</f>
@@ -2834,7 +2837,7 @@
       <c r="F23" s="95"/>
       <c r="G23" s="95"/>
       <c r="I23" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J23" s="85"/>
     </row>
@@ -2852,7 +2855,7 @@
       <c r="F24" s="95"/>
       <c r="G24" s="95"/>
       <c r="I24" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J24" s="85"/>
     </row>
@@ -2870,7 +2873,7 @@
       <c r="F25" s="95"/>
       <c r="G25" s="95"/>
       <c r="I25" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J25" s="85"/>
     </row>
@@ -2888,7 +2891,7 @@
       <c r="F26" s="95"/>
       <c r="G26" s="95"/>
       <c r="I26" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J26" s="85"/>
     </row>
@@ -2906,7 +2909,7 @@
       <c r="F27" s="95"/>
       <c r="G27" s="95"/>
       <c r="I27" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J27" s="85"/>
     </row>
@@ -2924,7 +2927,7 @@
       <c r="F28" s="95"/>
       <c r="G28" s="95"/>
       <c r="I28" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J28" s="85"/>
     </row>
@@ -2942,7 +2945,7 @@
       <c r="F29" s="95"/>
       <c r="G29" s="95"/>
       <c r="I29" s="133" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J29" s="85"/>
     </row>
@@ -2960,17 +2963,17 @@
       <c r="F30" s="95"/>
       <c r="G30" s="95"/>
       <c r="I30" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J30" s="85"/>
     </row>
     <row r="31" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B31" s="84"/>
       <c r="C31" s="146" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D31" s="97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E31" s="98">
         <v>4.5</v>
@@ -2978,17 +2981,17 @@
       <c r="F31" s="95"/>
       <c r="G31" s="95"/>
       <c r="I31" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J31" s="85"/>
     </row>
     <row r="32" spans="2:10" ht="16" customHeight="1" thickBot="1">
       <c r="B32" s="84"/>
       <c r="C32" s="146" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D32" s="97" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E32" s="98">
         <f>E31/E12</f>
@@ -2997,7 +3000,7 @@
       <c r="F32" s="95"/>
       <c r="G32" s="95"/>
       <c r="I32" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J32" s="85"/>
     </row>
@@ -3030,7 +3033,7 @@
       <c r="F35" s="95"/>
       <c r="G35" s="95"/>
       <c r="I35" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J35" s="85"/>
     </row>
@@ -3049,7 +3052,7 @@
       <c r="F36" s="95"/>
       <c r="G36" s="95"/>
       <c r="I36" s="147" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J36" s="85"/>
     </row>
@@ -3087,7 +3090,7 @@
       <c r="F38" s="95"/>
       <c r="G38" s="95"/>
       <c r="I38" s="147" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J38" s="85"/>
     </row>
@@ -3119,7 +3122,7 @@
   <dimension ref="B1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
@@ -3207,7 +3210,7 @@
       <c r="G6" s="41"/>
       <c r="H6" s="40"/>
       <c r="I6" s="126" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J6" s="68"/>
     </row>
@@ -3217,7 +3220,7 @@
         <v>69</v>
       </c>
       <c r="D7" s="143" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="137">
         <f>Notes!F16</f>
@@ -3227,7 +3230,7 @@
       <c r="G7" s="41"/>
       <c r="H7" s="40"/>
       <c r="I7" s="126" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J7" s="68"/>
     </row>
@@ -3247,7 +3250,7 @@
       <c r="G8" s="41"/>
       <c r="H8" s="40"/>
       <c r="I8" s="126" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J8" s="68"/>
     </row>
@@ -3260,14 +3263,14 @@
         <v>39</v>
       </c>
       <c r="E9" s="137">
-        <f>AVERAGE(Notes!E15:F15)</f>
-        <v>190</v>
+        <f>E8</f>
+        <v>380</v>
       </c>
       <c r="F9" s="41"/>
       <c r="G9" s="41"/>
       <c r="H9" s="40"/>
       <c r="I9" s="126" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="J9" s="68"/>
     </row>
@@ -3287,7 +3290,7 @@
       <c r="G10" s="41"/>
       <c r="H10" s="40"/>
       <c r="I10" s="126" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J10" s="68"/>
     </row>
@@ -3317,10 +3320,10 @@
     <row r="13" spans="2:10" ht="17" thickBot="1">
       <c r="B13" s="38"/>
       <c r="C13" s="145" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="143" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="132">
         <f>AVERAGE(Notes!E12:F12)</f>
@@ -3330,17 +3333,17 @@
       <c r="G13" s="41"/>
       <c r="H13" s="40"/>
       <c r="I13" s="126" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J13" s="68"/>
     </row>
     <row r="14" spans="2:10" ht="17" thickBot="1">
       <c r="B14" s="38"/>
       <c r="C14" s="145" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" s="143" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E14" s="129">
         <f>Notes!F13</f>
@@ -3350,7 +3353,7 @@
       <c r="G14" s="41"/>
       <c r="H14" s="40"/>
       <c r="I14" s="126" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J14" s="68"/>
     </row>
@@ -3393,7 +3396,7 @@
       <c r="G17" s="41"/>
       <c r="H17" s="40"/>
       <c r="I17" s="126" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J17" s="68"/>
     </row>
@@ -3490,7 +3493,7 @@
         <v>63</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J5" s="31" t="s">
         <v>64</v>
@@ -3507,13 +3510,13 @@
     </row>
     <row r="8" spans="2:11">
       <c r="C8" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="21" t="s">
         <v>94</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>95</v>
       </c>
       <c r="G8" s="125">
         <v>44562</v>
@@ -3528,7 +3531,7 @@
         <v>4</v>
       </c>
       <c r="K8" s="134" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="2:11">
@@ -3559,7 +3562,7 @@
   <dimension ref="B2:K166"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
@@ -3600,10 +3603,10 @@
         <v>58</v>
       </c>
       <c r="E4" s="109" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="109" t="s">
         <v>81</v>
-      </c>
-      <c r="F4" s="109" t="s">
-        <v>82</v>
       </c>
       <c r="G4" s="109" t="s">
         <v>10</v>
@@ -3639,10 +3642,10 @@
     <row r="7" spans="2:11">
       <c r="B7" s="14"/>
       <c r="C7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="141" t="s">
         <v>78</v>
-      </c>
-      <c r="D7" s="141" t="s">
-        <v>79</v>
       </c>
       <c r="E7" s="135"/>
       <c r="F7" s="135"/>
@@ -3668,7 +3671,7 @@
       <c r="B9" s="14"/>
       <c r="C9" s="12"/>
       <c r="D9" s="141" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" s="141">
         <v>160</v>
@@ -3708,7 +3711,7 @@
       <c r="B11" s="14"/>
       <c r="C11" s="12"/>
       <c r="D11" s="141" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="141" t="s">
         <v>4</v>
@@ -3728,7 +3731,7 @@
       <c r="B12" s="14"/>
       <c r="C12" s="12"/>
       <c r="D12" s="141" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12" s="141">
         <v>600000</v>
@@ -3737,7 +3740,7 @@
         <v>800000</v>
       </c>
       <c r="G12" s="141" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H12" s="142"/>
       <c r="I12" s="141"/>
@@ -3748,7 +3751,7 @@
       <c r="B13" s="14"/>
       <c r="C13" s="12"/>
       <c r="D13" s="141" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E13" s="141" t="s">
         <v>4</v>
@@ -3757,10 +3760,10 @@
         <v>50000</v>
       </c>
       <c r="G13" s="141" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H13" s="142" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I13" s="141"/>
       <c r="J13" s="141"/>
@@ -3770,7 +3773,7 @@
       <c r="B14" s="14"/>
       <c r="C14" s="12"/>
       <c r="D14" s="141" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E14" s="141" t="s">
         <v>4</v>
@@ -3790,7 +3793,7 @@
       <c r="B15" s="14"/>
       <c r="C15" s="12"/>
       <c r="D15" s="141" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" s="141">
         <v>80</v>
@@ -3810,7 +3813,7 @@
       <c r="B16" s="14"/>
       <c r="C16" s="12"/>
       <c r="D16" s="141" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E16" s="141" t="s">
         <v>4</v>
@@ -3819,10 +3822,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="141" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H16" s="142" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I16" s="141"/>
       <c r="J16" s="141"/>
@@ -3832,7 +3835,7 @@
       <c r="B17" s="14"/>
       <c r="C17" s="12"/>
       <c r="D17" s="152" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" s="152">
         <v>15</v>
@@ -3841,10 +3844,10 @@
         <v>100</v>
       </c>
       <c r="G17" s="152" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H17" s="153" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I17" s="141"/>
       <c r="J17" s="141"/>
@@ -3873,7 +3876,7 @@
       <c r="B20" s="14"/>
       <c r="C20" s="12"/>
       <c r="D20" s="152" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E20" s="152">
         <v>1</v>
@@ -3886,7 +3889,7 @@
         <v>4</v>
       </c>
       <c r="H20" s="153" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I20" s="141"/>
       <c r="J20" s="141"/>

</xml_diff>